<commit_message>
Framework A2 First Commit
</commit_message>
<xml_diff>
--- a/src/test/resources/Test Data.xlsx
+++ b/src/test/resources/Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konik\eclipse-workspace\SkillraryDemoApp\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0FAB38-40CF-4B17-84ED-7A1047943483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0829F64-2225-4D18-883A-47922E2D27C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B282D014-781E-4B72-8398-6673E2986076}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>TC_ID</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>C:\Users\konik\Downloads\oie_315151ckg7CGB2.jpg</t>
   </si>
   <si>
@@ -135,10 +132,13 @@
     <t>Koniki</t>
   </si>
   <si>
-    <t>Selenium Testing987</t>
-  </si>
-  <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>selenium Testing987</t>
   </si>
 </sst>
 </file>
@@ -600,7 +600,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -608,7 +608,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -616,7 +616,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -624,7 +624,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -648,12 +648,12 @@
         <v>13</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C9" t="s" s="0">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -684,7 +684,7 @@
         <v>17</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -692,7 +692,7 @@
         <v>18</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -708,20 +708,20 @@
         <v>13</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C15" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s" s="0">
         <v>22</v>
-      </c>
-      <c r="D15" t="s" s="0">
-        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C16" t="s" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -743,24 +743,24 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s" s="0">
         <v>17</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" t="s" s="0">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C19" t="s" s="0">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>